<commit_message>
Cells are still locked on downloading. I simply unlocked everything
</commit_message>
<xml_diff>
--- a/Excel_References_example.xlsx
+++ b/Excel_References_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/ennowinkler_ennosgermancourse_onmicrosoft_com/Documents/excelbib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_FCABCD9777D094EC5F730EC0997A9122F62C3D7E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74052C3D-D97B-4745-8A35-26CE7776ACE6}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_FCABCD9777D094EC5F730EC0997A9122F62C3D7E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1651735-4185-4B2F-B41F-B70C57A5F16E}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17297,7 +17297,7 @@
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B5" sqref="B5"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33522,10 +33522,6 @@
       </c>
     </row>
   </sheetData>
-  <protectedRanges>
-    <protectedRange sqref="I1:CF1048576" name="Range2"/>
-    <protectedRange sqref="A1:A1048576" name="Range1"/>
-  </protectedRanges>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>